<commit_message>
Updated analysed sessions Nathan
</commit_message>
<xml_diff>
--- a/src/visualpipe/post_analysis/Nathan_sessions.xlsx
+++ b/src/visualpipe/post_analysis/Nathan_sessions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mai-an.nguyen\Work\VISUALPIPE\src\visualpipe\post_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://instituteicm-my.sharepoint.com/personal/nathan_mallet_icm-institute_org/Documents/Documents/GitHub/VISUALPIPE/src/visualpipe/post_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A12C356-FC54-474C-9FEE-4837ACE482B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{8A12C356-FC54-474C-9FEE-4837ACE482B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E056CA95-A54D-4328-A80A-6B411E85C41D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{65663A8A-8BAF-40AD-BE50-4073098D8478}"/>
+    <workbookView xWindow="5865" yWindow="1770" windowWidth="20400" windowHeight="14535" xr2:uid="{65663A8A-8BAF-40AD-BE50-4073098D8478}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Session_id</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>2025_03_03_17-14-33</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>dt_post_stim is 0</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -242,6 +248,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3249E33-83F8-4F23-B204-609515E16092}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +603,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,13 +625,16 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -639,13 +651,16 @@
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -662,13 +677,16 @@
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -685,13 +703,16 @@
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -708,13 +729,16 @@
       <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -731,13 +755,16 @@
       <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -754,13 +781,16 @@
       <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -777,13 +807,16 @@
       <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -800,8 +833,11 @@
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -824,7 +860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -847,7 +883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -870,7 +906,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -893,7 +929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -916,7 +952,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -938,6 +974,9 @@
       <c r="G15" s="1" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add neuron_type to excel sheet
</commit_message>
<xml_diff>
--- a/src/visualpipe/post_analysis/Nathan_sessions.xlsx
+++ b/src/visualpipe/post_analysis/Nathan_sessions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://instituteicm-my.sharepoint.com/personal/nathan_mallet_icm-institute_org/Documents/Documents/GitHub/VISUALPIPE/src/visualpipe/post_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mai-an.nguyen\Work\VISUALPIPE\src\visualpipe\post_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{8A12C356-FC54-474C-9FEE-4837ACE482B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E056CA95-A54D-4328-A80A-6B411E85C41D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041C3B0-460B-49E6-B1D9-92B247DADB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="1770" windowWidth="20400" windowHeight="14535" xr2:uid="{65663A8A-8BAF-40AD-BE50-4073098D8478}"/>
+    <workbookView xWindow="38280" yWindow="-555" windowWidth="29040" windowHeight="17640" xr2:uid="{65663A8A-8BAF-40AD-BE50-4073098D8478}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t>Session_id</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>dt_post_stim is 0</t>
+  </si>
+  <si>
+    <t>Neuron_type</t>
+  </si>
+  <si>
+    <t>PYR</t>
   </si>
 </sst>
 </file>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3249E33-83F8-4F23-B204-609515E16092}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F2" sqref="F2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,11 +605,12 @@
     <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,16 +627,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -645,17 +655,20 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -671,17 +684,20 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -697,17 +713,20 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -723,17 +742,20 @@
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -749,17 +771,20 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -775,17 +800,20 @@
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -801,17 +829,20 @@
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -827,17 +858,20 @@
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -853,14 +887,17 @@
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -876,14 +913,17 @@
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -899,14 +939,17 @@
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -922,14 +965,17 @@
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -945,14 +991,17 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -968,10 +1017,13 @@
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>